<commit_message>
Incorporated examples for fields within nested objects/structures.
</commit_message>
<xml_diff>
--- a/Assets/Basic/Data/Example.xlsx
+++ b/Assets/Basic/Data/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\excel-2-unity-example\Assets\Basic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F594A0-20A9-4F39-BD1F-4DDFAF05CB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64E3987-1DD0-419A-BC17-23A05C6D4B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25110" yWindow="3675" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExampleConstants" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="531">
   <si>
     <t>Name</t>
   </si>
@@ -1320,9 +1320,6 @@
 676</t>
   </si>
   <si>
-    <t>[{"id":HERO_1, "name":"John Doe 1"},{"id":HERO_2, "name":"Mary Sue 2"}]</t>
-  </si>
-  <si>
     <t>text1 | text4</t>
   </si>
   <si>
@@ -1707,13 +1704,82 @@
   </si>
   <si>
     <t xml:space="preserve">Vector3 example </t>
+  </si>
+  <si>
+    <t>currency.coin.min</t>
+  </si>
+  <si>
+    <t>currency.coin.max</t>
+  </si>
+  <si>
+    <t>character.name</t>
+  </si>
+  <si>
+    <t>character.sex</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Hanoi</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>currency.gemMin</t>
+  </si>
+  <si>
+    <t>currency.gemMax</t>
+  </si>
+  <si>
+    <t>10 | 20 | 30 | 50</t>
+  </si>
+  <si>
+    <t>11 | 20 | 30 | 50</t>
+  </si>
+  <si>
+    <t>12 | 20 | 30 | 50</t>
+  </si>
+  <si>
+    <t>13 | 20 | 30 | 50</t>
+  </si>
+  <si>
+    <t>14 | 20 | 30 | 50</t>
+  </si>
+  <si>
+    <t>15 | 20 | 30 | 50</t>
+  </si>
+  <si>
+    <t>16 | 20 | 30 | 50</t>
+  </si>
+  <si>
+    <t>{"name": [ "english", "spansih", "japanese"]}</t>
+  </si>
+  <si>
+    <t>nestedArray.examples[]</t>
+  </si>
+  <si>
+    <t>nestedJson.examples{}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1763,6 +1829,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1970,6 +2042,12 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1978,12 +2056,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2590,7 +2662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -2627,8 +2699,8 @@
       <c r="C2" s="35">
         <v>83</v>
       </c>
-      <c r="D2" s="42" t="s">
-        <v>504</v>
+      <c r="D2" s="39" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2641,8 +2713,8 @@
       <c r="C3" s="35">
         <v>1.0209999999999999</v>
       </c>
-      <c r="D3" s="42" t="s">
-        <v>506</v>
+      <c r="D3" s="39" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2655,8 +2727,8 @@
       <c r="C4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>505</v>
+      <c r="D4" s="39" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2672,8 +2744,8 @@
       <c r="C6" s="38">
         <v>4</v>
       </c>
-      <c r="D6" s="43" t="s">
-        <v>502</v>
+      <c r="D6" s="40" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2686,8 +2758,8 @@
       <c r="C7" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="43" t="s">
-        <v>502</v>
+      <c r="D7" s="40" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2703,8 +2775,8 @@
       <c r="C9" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>503</v>
+      <c r="D9" s="39" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2717,8 +2789,8 @@
       <c r="C10" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>503</v>
+      <c r="D10" s="39" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2734,8 +2806,8 @@
       <c r="C12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="43" t="s">
-        <v>507</v>
+      <c r="D12" s="40" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2748,8 +2820,8 @@
       <c r="C13" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="43" t="s">
-        <v>507</v>
+      <c r="D13" s="40" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2762,8 +2834,8 @@
       <c r="C14" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="43" t="s">
-        <v>508</v>
+      <c r="D14" s="40" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2779,8 +2851,8 @@
       <c r="C16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="42" t="s">
-        <v>502</v>
+      <c r="D16" s="39" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2793,8 +2865,8 @@
       <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="42" t="s">
-        <v>502</v>
+      <c r="D17" s="39" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2808,7 +2880,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30">
@@ -2837,7 +2909,7 @@
         <v>360</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2852,7 +2924,7 @@
         <v>45</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2866,7 +2938,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3838,7 +3910,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="41" t="s">
         <v>187</v>
       </c>
       <c r="B20" s="15" t="s">
@@ -3864,7 +3936,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="39"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="15" t="s">
         <v>51</v>
       </c>
@@ -3888,7 +3960,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="39"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="15" t="s">
         <v>57</v>
       </c>
@@ -3912,7 +3984,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="39"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="15" t="s">
         <v>63</v>
       </c>
@@ -3936,7 +4008,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="39"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="15" t="s">
         <v>69</v>
       </c>
@@ -4030,31 +4102,31 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
@@ -4073,12 +4145,12 @@
         <v>223</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
@@ -4097,12 +4169,12 @@
         <v>228</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10" t="s">
@@ -4121,12 +4193,12 @@
         <v>233</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
@@ -4145,12 +4217,12 @@
         <v>238</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
@@ -4169,12 +4241,12 @@
         <v>243</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10" t="s">
@@ -4193,12 +4265,12 @@
         <v>248</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
@@ -4217,12 +4289,12 @@
         <v>253</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10" t="s">
@@ -4241,12 +4313,12 @@
         <v>258</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
@@ -4265,12 +4337,12 @@
         <v>263</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10" t="s">
@@ -4289,12 +4361,12 @@
         <v>268</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
@@ -4313,12 +4385,12 @@
         <v>273</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
@@ -4337,12 +4409,12 @@
         <v>278</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
@@ -4366,7 +4438,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
@@ -4385,12 +4457,12 @@
         <v>287</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
@@ -4409,12 +4481,12 @@
         <v>292</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
@@ -4433,12 +4505,12 @@
         <v>297</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
@@ -4457,12 +4529,12 @@
         <v>302</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
@@ -4481,12 +4553,12 @@
         <v>307</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
@@ -4505,12 +4577,12 @@
         <v>312</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
@@ -4529,12 +4601,12 @@
         <v>317</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
@@ -4553,12 +4625,12 @@
         <v>322</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
@@ -4577,12 +4649,12 @@
         <v>327</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
@@ -4601,12 +4673,12 @@
         <v>332</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30">
       <c r="A26" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
@@ -4625,12 +4697,12 @@
         <v>337</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
@@ -4649,7 +4721,7 @@
         <v>342</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -4660,10 +4732,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4671,9 +4743,17 @@
     <col min="1" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>343</v>
       </c>
@@ -4689,8 +4769,26 @@
       <c r="E1" s="3" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4706,8 +4804,28 @@
       <c r="E2" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="20">
+        <v>10</v>
+      </c>
+      <c r="G2" s="20">
+        <f>F2*2</f>
+        <v>20</v>
+      </c>
+      <c r="H2" s="20">
+        <v>1</v>
+      </c>
+      <c r="I2" s="20">
+        <f>H2*2</f>
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4723,8 +4841,28 @@
       <c r="E3" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="20">
+        <v>20</v>
+      </c>
+      <c r="G3" s="20">
+        <f t="shared" ref="G3:I8" si="0">F3*2</f>
+        <v>40</v>
+      </c>
+      <c r="H3" s="20">
+        <v>2</v>
+      </c>
+      <c r="I3" s="20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4740,8 +4878,28 @@
       <c r="E4" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="20">
+        <v>30</v>
+      </c>
+      <c r="G4" s="20">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H4" s="20">
+        <v>3</v>
+      </c>
+      <c r="I4" s="20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4">
         <v>6</v>
       </c>
@@ -4757,8 +4915,28 @@
       <c r="E5" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="20">
+        <v>40</v>
+      </c>
+      <c r="G5" s="20">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H5" s="20">
+        <v>4</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="4">
         <v>9</v>
       </c>
@@ -4774,9 +4952,29 @@
       <c r="E6" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="40">
+      <c r="F6" s="20">
+        <v>50</v>
+      </c>
+      <c r="G6" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H6" s="20">
+        <v>5</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="42">
         <v>14</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -4791,9 +4989,29 @@
       <c r="E7" s="9" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="40"/>
+      <c r="F7" s="20">
+        <v>60</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="H7" s="20">
+        <v>6</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="42"/>
       <c r="B8" s="9" t="s">
         <v>83</v>
       </c>
@@ -4805,22 +5023,43 @@
       </c>
       <c r="E8" s="9" t="s">
         <v>348</v>
+      </c>
+      <c r="F8" s="20">
+        <v>70</v>
+      </c>
+      <c r="G8" s="20">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="H8" s="20">
+        <v>7</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A7:A8"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="15"/>
@@ -4831,9 +5070,10 @@
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="6" width="7.85546875" customWidth="1"/>
     <col min="7" max="7" width="68.7109375" customWidth="1"/>
+    <col min="9" max="9" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>349</v>
       </c>
@@ -4855,8 +5095,14 @@
       <c r="G1" s="3" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30">
+      <c r="H1" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="8" t="s">
         <v>356</v>
       </c>
@@ -4878,8 +5124,14 @@
       <c r="G2" s="9" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30">
+      <c r="H2" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" s="4" t="s">
         <v>360</v>
       </c>
@@ -4901,8 +5153,14 @@
       <c r="G3" s="9" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30">
+      <c r="H3" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="8" t="s">
         <v>366</v>
       </c>
@@ -4924,8 +5182,14 @@
       <c r="G4" s="9" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30">
+      <c r="H4" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" s="8" t="s">
         <v>372</v>
       </c>
@@ -4947,8 +5211,14 @@
       <c r="G5" s="9" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
+      <c r="H5" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" s="4" t="s">
         <v>376</v>
       </c>
@@ -4968,15 +5238,21 @@
         <v>358</v>
       </c>
       <c r="G6" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="4" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>381</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>382</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>362</v>
@@ -4985,36 +5261,48 @@
         <v>363</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>358</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
+        <v>359</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B8" s="4">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>358</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>380</v>
+        <v>359</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -5055,61 +5343,61 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>404</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -5117,7 +5405,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>49</v>
@@ -5152,7 +5440,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>84</v>
@@ -5195,7 +5483,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>72</v>
@@ -5216,16 +5504,16 @@
         <v>91</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>412</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>55</v>
@@ -5248,7 +5536,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>55</v>
@@ -5269,16 +5557,16 @@
         <v>91</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>416</v>
-      </c>
       <c r="L5" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>55</v>
@@ -5305,7 +5593,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>84</v>
@@ -5344,7 +5632,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>49</v>
@@ -5385,7 +5673,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -5435,46 +5723,46 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>430</v>
-      </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="41">
+      <c r="A2" s="43">
         <v>100</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="43">
         <v>200</v>
       </c>
       <c r="C2" s="1">
@@ -5494,25 +5782,25 @@
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I2" s="1">
         <v>12</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="1">
         <v>4</v>
       </c>
@@ -5522,8 +5810,8 @@
       <c r="E3" s="1">
         <v>6</v>
       </c>
-      <c r="F3" s="41" t="s">
-        <v>434</v>
+      <c r="F3" s="43" t="s">
+        <v>433</v>
       </c>
       <c r="G3" s="1">
         <f>AVERAGE(C3:E3)</f>
@@ -5537,21 +5825,21 @@
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L3" s="2">
         <v>2</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="41"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="43">
         <v>500</v>
       </c>
       <c r="D4" s="1">
@@ -5560,40 +5848,40 @@
       <c r="E4" s="1">
         <v>7</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="43"/>
       <c r="G4" s="1">
         <v>3</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I4" s="1">
         <v>4</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L4" s="2">
         <v>3</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="41"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="1">
         <v>5</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="1">
         <v>7</v>
       </c>
       <c r="E5" s="1">
         <v>8</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="43"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2" t="s">
         <v>218</v>
@@ -5603,17 +5891,17 @@
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L5" s="2">
         <v>4</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="41"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="1">
         <v>6</v>
       </c>
@@ -5626,23 +5914,23 @@
       <c r="E6" s="1">
         <v>9</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I6" s="1">
         <v>6</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L6" s="2">
         <v>5</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -5673,13 +5961,13 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="L7" s="2">
         <v>6</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>